<commit_message>
updating the xlsx tool
</commit_message>
<xml_diff>
--- a/input/tool/SurveyTool.xlsx
+++ b/input/tool/SurveyTool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wfp-my.sharepoint.com/personal/ahmed_mohamoud_wfp_org/Documents/6_Git_Projects/Ahmed_Project/input/tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="8_{B8F20A3A-BA69-4798-A3F5-6AE7D3A16E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{836B5188-0D22-4239-B562-7B5F1A8309ED}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="8_{B8F20A3A-BA69-4798-A3F5-6AE7D3A16E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3991CDDF-0D69-4471-B127-CF02B1EEE4BC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB73E7E0-20D7-4C43-972D-5164B2FE7CBB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DB73E7E0-20D7-4C43-972D-5164B2FE7CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>today</t>
   </si>
   <si>
-    <t>relevent</t>
-  </si>
-  <si>
     <t>required</t>
   </si>
   <si>
@@ -1516,6 +1513,9 @@
   </si>
   <si>
     <t>badhan</t>
+  </si>
+  <si>
+    <t>relevant</t>
   </si>
 </sst>
 </file>
@@ -1903,7 +1903,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1931,28 +1931,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
@@ -1989,13 +1989,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2008,40 +2008,40 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7" t="s">
         <v>266</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>267</v>
-      </c>
-      <c r="C7" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B8" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" t="s">
         <v>270</v>
-      </c>
-      <c r="C8" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2056,13 +2056,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -2075,73 +2075,73 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2156,13 +2156,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -2175,73 +2175,73 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
         <v>82</v>
-      </c>
-      <c r="C20" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
         <v>84</v>
-      </c>
-      <c r="C21" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
         <v>86</v>
-      </c>
-      <c r="C22" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" t="s">
         <v>88</v>
-      </c>
-      <c r="C23" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
         <v>90</v>
-      </c>
-      <c r="C24" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" t="s">
         <v>92</v>
-      </c>
-      <c r="C25" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2256,13 +2256,13 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -2275,851 +2275,851 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" t="s">
         <v>112</v>
       </c>
-      <c r="C29" t="s">
-        <v>113</v>
-      </c>
       <c r="F29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" t="s">
         <v>133</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>134</v>
-      </c>
-      <c r="C30" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" t="s">
         <v>136</v>
-      </c>
-      <c r="C31" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B32" t="s">
         <v>138</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>139</v>
       </c>
-      <c r="C32" t="s">
-        <v>140</v>
-      </c>
       <c r="K32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B33" t="s">
+        <v>140</v>
+      </c>
+      <c r="C33" t="s">
         <v>141</v>
       </c>
-      <c r="C33" t="s">
-        <v>142</v>
-      </c>
       <c r="K33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" t="s">
         <v>114</v>
       </c>
-      <c r="C35" t="s">
-        <v>115</v>
-      </c>
       <c r="F35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C38" t="s">
         <v>146</v>
       </c>
-      <c r="C38" t="s">
-        <v>147</v>
-      </c>
       <c r="K38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" t="s">
         <v>116</v>
       </c>
-      <c r="C40" t="s">
-        <v>117</v>
-      </c>
       <c r="F40" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C43" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B45" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45" t="s">
         <v>118</v>
       </c>
-      <c r="C45" t="s">
-        <v>119</v>
-      </c>
       <c r="F45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K45" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" t="s">
         <v>155</v>
       </c>
-      <c r="C48" t="s">
-        <v>156</v>
-      </c>
       <c r="F48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K50" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" t="s">
         <v>160</v>
       </c>
-      <c r="C52" t="s">
-        <v>161</v>
-      </c>
       <c r="F52" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K52" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C53" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K54" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" t="s">
         <v>165</v>
       </c>
-      <c r="C56" t="s">
-        <v>166</v>
-      </c>
       <c r="F56" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K56" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B58" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K58" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B60" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" t="s">
         <v>170</v>
       </c>
-      <c r="C60" t="s">
-        <v>171</v>
-      </c>
       <c r="F60" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B62" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C62" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B63" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B64" t="s">
+        <v>119</v>
+      </c>
+      <c r="C64" t="s">
         <v>120</v>
       </c>
-      <c r="C64" t="s">
-        <v>121</v>
-      </c>
       <c r="F64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K64" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C65" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B67" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" t="s">
         <v>177</v>
       </c>
-      <c r="C67" t="s">
-        <v>178</v>
-      </c>
       <c r="F67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K67" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B68" t="s">
+        <v>178</v>
+      </c>
+      <c r="C68" t="s">
         <v>179</v>
       </c>
-      <c r="C68" t="s">
-        <v>180</v>
-      </c>
       <c r="F68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K68" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B69" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C69" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K70" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B71" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B72" t="s">
+        <v>121</v>
+      </c>
+      <c r="C72" t="s">
         <v>122</v>
       </c>
-      <c r="C72" t="s">
-        <v>123</v>
-      </c>
       <c r="F72" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K72" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B73" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B74" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B75" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" t="s">
         <v>186</v>
       </c>
-      <c r="C75" t="s">
-        <v>187</v>
-      </c>
       <c r="F75" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K75" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B77" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C77" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K77" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B78" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C78" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B79" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" t="s">
         <v>124</v>
       </c>
-      <c r="C79" t="s">
-        <v>125</v>
-      </c>
       <c r="F79" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K79" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B80" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B81" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C81" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B82" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C82" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K82" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B83" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C83" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B84" t="s">
+        <v>125</v>
+      </c>
+      <c r="C84" t="s">
         <v>126</v>
       </c>
-      <c r="C84" t="s">
-        <v>127</v>
-      </c>
       <c r="F84" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K84" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B85" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C85" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B86" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C86" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B87" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C87" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K87" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B88" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C88" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B89" t="s">
+        <v>127</v>
+      </c>
+      <c r="C89" t="s">
         <v>128</v>
       </c>
-      <c r="C89" t="s">
-        <v>129</v>
-      </c>
       <c r="F89" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="K89" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B90" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B91" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C91" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C92" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K92" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -3134,13 +3134,13 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -3153,73 +3153,73 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B95" t="s">
+        <v>251</v>
+      </c>
+      <c r="C95" t="s">
         <v>252</v>
-      </c>
-      <c r="C95" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B96" t="s">
+        <v>253</v>
+      </c>
+      <c r="C96" t="s">
         <v>254</v>
-      </c>
-      <c r="C96" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B97" t="s">
+        <v>255</v>
+      </c>
+      <c r="C97" t="s">
         <v>256</v>
-      </c>
-      <c r="C97" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B98" t="s">
+        <v>257</v>
+      </c>
+      <c r="C98" t="s">
         <v>258</v>
-      </c>
-      <c r="C98" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B99" t="s">
+        <v>259</v>
+      </c>
+      <c r="C99" t="s">
         <v>260</v>
-      </c>
-      <c r="C99" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B100" t="s">
+        <v>261</v>
+      </c>
+      <c r="C100" t="s">
         <v>262</v>
-      </c>
-      <c r="C100" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -3234,13 +3234,13 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>265</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -3276,7 +3276,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3287,343 +3287,343 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
         <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" t="s">
         <v>95</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>96</v>
-      </c>
-      <c r="C29" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
         <v>98</v>
-      </c>
-      <c r="C30" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
         <v>100</v>
-      </c>
-      <c r="C31" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" t="s">
         <v>102</v>
-      </c>
-      <c r="C32" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" t="s">
         <v>104</v>
-      </c>
-      <c r="C33" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" t="s">
         <v>106</v>
-      </c>
-      <c r="C34" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B36" s="4">
         <v>0</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -3631,1465 +3631,1465 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B39" s="4">
         <v>100</v>
       </c>
       <c r="C39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B40" s="4">
         <v>1000</v>
       </c>
       <c r="C40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B41" s="4">
         <v>1001</v>
       </c>
       <c r="C41" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B42" s="4">
         <v>1002</v>
       </c>
       <c r="C42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B43" s="4">
         <v>1003</v>
       </c>
       <c r="C43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B44" s="4">
         <v>101</v>
       </c>
       <c r="C44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B45" s="4">
         <v>102</v>
       </c>
       <c r="C45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B46" s="4">
         <v>200</v>
       </c>
       <c r="C46" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B47" s="4">
         <v>300</v>
       </c>
       <c r="C47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B48" s="4">
         <v>400</v>
       </c>
       <c r="C48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B49" s="4">
         <v>500</v>
       </c>
       <c r="C49" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B50" s="4">
         <v>501</v>
       </c>
       <c r="C50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B51" s="4">
         <v>502</v>
       </c>
       <c r="C51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B52" s="4">
         <v>503</v>
       </c>
       <c r="C52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B53" s="4">
         <v>504</v>
       </c>
       <c r="C53" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B54" s="4">
         <v>600</v>
       </c>
       <c r="C54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B55" s="4">
         <v>700</v>
       </c>
       <c r="C55" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B56" s="4">
         <v>800</v>
       </c>
       <c r="C56" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B57" s="4">
         <v>801</v>
       </c>
       <c r="C57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B58" s="4">
         <v>802</v>
       </c>
       <c r="C58" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B59" s="4">
         <v>900</v>
       </c>
       <c r="C59" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B60" s="4">
         <v>999</v>
       </c>
       <c r="C60" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B62" t="s">
+        <v>273</v>
+      </c>
+      <c r="C62" t="s">
         <v>274</v>
-      </c>
-      <c r="C62" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B63" t="s">
+        <v>275</v>
+      </c>
+      <c r="C63" t="s">
         <v>276</v>
-      </c>
-      <c r="C63" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B64" t="s">
+        <v>277</v>
+      </c>
+      <c r="C64" t="s">
         <v>278</v>
-      </c>
-      <c r="C64" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B65" t="s">
+        <v>279</v>
+      </c>
+      <c r="C65" t="s">
         <v>280</v>
-      </c>
-      <c r="C65" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B66" t="s">
+        <v>281</v>
+      </c>
+      <c r="C66" t="s">
         <v>282</v>
-      </c>
-      <c r="C66" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B67" t="s">
+        <v>283</v>
+      </c>
+      <c r="C67" t="s">
         <v>284</v>
-      </c>
-      <c r="C67" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B68" t="s">
+        <v>285</v>
+      </c>
+      <c r="C68" t="s">
         <v>286</v>
-      </c>
-      <c r="C68" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B69" t="s">
+        <v>287</v>
+      </c>
+      <c r="C69" t="s">
         <v>288</v>
-      </c>
-      <c r="C69" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B70" t="s">
+        <v>289</v>
+      </c>
+      <c r="C70" t="s">
         <v>290</v>
-      </c>
-      <c r="C70" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B71" t="s">
+        <v>291</v>
+      </c>
+      <c r="C71" t="s">
         <v>292</v>
-      </c>
-      <c r="C71" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B72" t="s">
+        <v>293</v>
+      </c>
+      <c r="C72" t="s">
         <v>294</v>
-      </c>
-      <c r="C72" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B73" t="s">
+        <v>295</v>
+      </c>
+      <c r="C73" t="s">
         <v>296</v>
-      </c>
-      <c r="C73" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B74" t="s">
+        <v>297</v>
+      </c>
+      <c r="C74" t="s">
         <v>298</v>
-      </c>
-      <c r="C74" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B75" t="s">
+        <v>299</v>
+      </c>
+      <c r="C75" t="s">
         <v>300</v>
-      </c>
-      <c r="C75" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B76" t="s">
+        <v>301</v>
+      </c>
+      <c r="C76" t="s">
         <v>302</v>
-      </c>
-      <c r="C76" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B77" t="s">
+        <v>303</v>
+      </c>
+      <c r="C77" t="s">
         <v>304</v>
-      </c>
-      <c r="C77" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B78" t="s">
+        <v>305</v>
+      </c>
+      <c r="C78" t="s">
         <v>306</v>
-      </c>
-      <c r="C78" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B79" t="s">
+        <v>307</v>
+      </c>
+      <c r="C79" t="s">
         <v>308</v>
-      </c>
-      <c r="C79" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B81" t="s">
+        <v>309</v>
+      </c>
+      <c r="C81" t="s">
         <v>310</v>
-      </c>
-      <c r="C81" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B82" t="s">
+        <v>311</v>
+      </c>
+      <c r="C82" t="s">
         <v>312</v>
-      </c>
-      <c r="C82" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B83" t="s">
+        <v>313</v>
+      </c>
+      <c r="C83" t="s">
         <v>314</v>
-      </c>
-      <c r="C83" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B84" t="s">
+        <v>315</v>
+      </c>
+      <c r="C84" t="s">
         <v>316</v>
-      </c>
-      <c r="C84" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B85" t="s">
+        <v>317</v>
+      </c>
+      <c r="C85" t="s">
         <v>318</v>
-      </c>
-      <c r="C85" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B86" t="s">
+        <v>319</v>
+      </c>
+      <c r="C86" t="s">
         <v>320</v>
-      </c>
-      <c r="C86" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B87" t="s">
+        <v>321</v>
+      </c>
+      <c r="C87" t="s">
         <v>322</v>
-      </c>
-      <c r="C87" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B88" t="s">
+        <v>323</v>
+      </c>
+      <c r="C88" t="s">
         <v>324</v>
-      </c>
-      <c r="C88" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B89" t="s">
+        <v>325</v>
+      </c>
+      <c r="C89" t="s">
         <v>326</v>
-      </c>
-      <c r="C89" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B90" t="s">
+        <v>327</v>
+      </c>
+      <c r="C90" t="s">
         <v>328</v>
-      </c>
-      <c r="C90" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B91" t="s">
+        <v>329</v>
+      </c>
+      <c r="C91" t="s">
         <v>330</v>
-      </c>
-      <c r="C91" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B92" t="s">
+        <v>331</v>
+      </c>
+      <c r="C92" t="s">
         <v>332</v>
-      </c>
-      <c r="C92" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B93" t="s">
+        <v>333</v>
+      </c>
+      <c r="C93" t="s">
         <v>334</v>
-      </c>
-      <c r="C93" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B94" t="s">
+        <v>335</v>
+      </c>
+      <c r="C94" t="s">
         <v>336</v>
-      </c>
-      <c r="C94" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B95" t="s">
+        <v>337</v>
+      </c>
+      <c r="C95" t="s">
         <v>338</v>
-      </c>
-      <c r="C95" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B96" t="s">
+        <v>339</v>
+      </c>
+      <c r="C96" t="s">
         <v>340</v>
-      </c>
-      <c r="C96" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B97" t="s">
+        <v>341</v>
+      </c>
+      <c r="C97" t="s">
         <v>342</v>
-      </c>
-      <c r="C97" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B98" t="s">
+        <v>343</v>
+      </c>
+      <c r="C98" t="s">
         <v>344</v>
-      </c>
-      <c r="C98" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B99" t="s">
+        <v>345</v>
+      </c>
+      <c r="C99" t="s">
         <v>346</v>
-      </c>
-      <c r="C99" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B100" t="s">
+        <v>347</v>
+      </c>
+      <c r="C100" t="s">
         <v>348</v>
-      </c>
-      <c r="C100" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B101" t="s">
+        <v>349</v>
+      </c>
+      <c r="C101" t="s">
         <v>350</v>
-      </c>
-      <c r="C101" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B102" t="s">
+        <v>351</v>
+      </c>
+      <c r="C102" t="s">
         <v>352</v>
-      </c>
-      <c r="C102" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B103" t="s">
+        <v>353</v>
+      </c>
+      <c r="C103" t="s">
         <v>354</v>
-      </c>
-      <c r="C103" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B104" t="s">
+        <v>355</v>
+      </c>
+      <c r="C104" t="s">
         <v>356</v>
-      </c>
-      <c r="C104" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B105" t="s">
+        <v>357</v>
+      </c>
+      <c r="C105" t="s">
         <v>358</v>
-      </c>
-      <c r="C105" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B106" t="s">
+        <v>359</v>
+      </c>
+      <c r="C106" t="s">
         <v>360</v>
-      </c>
-      <c r="C106" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B107" t="s">
+        <v>361</v>
+      </c>
+      <c r="C107" t="s">
         <v>362</v>
-      </c>
-      <c r="C107" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B108" t="s">
+        <v>363</v>
+      </c>
+      <c r="C108" t="s">
         <v>364</v>
-      </c>
-      <c r="C108" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B109" t="s">
+        <v>365</v>
+      </c>
+      <c r="C109" t="s">
         <v>366</v>
-      </c>
-      <c r="C109" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B110" t="s">
+        <v>367</v>
+      </c>
+      <c r="C110" t="s">
         <v>368</v>
-      </c>
-      <c r="C110" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B111" t="s">
+        <v>369</v>
+      </c>
+      <c r="C111" t="s">
         <v>370</v>
-      </c>
-      <c r="C111" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B112" t="s">
+        <v>371</v>
+      </c>
+      <c r="C112" t="s">
         <v>372</v>
-      </c>
-      <c r="C112" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B113" t="s">
+        <v>373</v>
+      </c>
+      <c r="C113" t="s">
         <v>374</v>
-      </c>
-      <c r="C113" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B114" t="s">
+        <v>375</v>
+      </c>
+      <c r="C114" t="s">
         <v>376</v>
-      </c>
-      <c r="C114" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B115" t="s">
+        <v>377</v>
+      </c>
+      <c r="C115" t="s">
         <v>378</v>
-      </c>
-      <c r="C115" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B116" t="s">
+        <v>379</v>
+      </c>
+      <c r="C116" t="s">
         <v>380</v>
-      </c>
-      <c r="C116" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B117" t="s">
+        <v>381</v>
+      </c>
+      <c r="C117" t="s">
         <v>382</v>
-      </c>
-      <c r="C117" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B118" t="s">
+        <v>383</v>
+      </c>
+      <c r="C118" t="s">
         <v>384</v>
-      </c>
-      <c r="C118" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B119" t="s">
+        <v>385</v>
+      </c>
+      <c r="C119" t="s">
         <v>386</v>
-      </c>
-      <c r="C119" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B120" t="s">
+        <v>387</v>
+      </c>
+      <c r="C120" t="s">
         <v>388</v>
-      </c>
-      <c r="C120" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B121" t="s">
+        <v>389</v>
+      </c>
+      <c r="C121" t="s">
         <v>390</v>
-      </c>
-      <c r="C121" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B122" t="s">
+        <v>391</v>
+      </c>
+      <c r="C122" t="s">
         <v>392</v>
-      </c>
-      <c r="C122" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B123" t="s">
+        <v>393</v>
+      </c>
+      <c r="C123" t="s">
         <v>394</v>
-      </c>
-      <c r="C123" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B124" t="s">
+        <v>395</v>
+      </c>
+      <c r="C124" t="s">
         <v>396</v>
-      </c>
-      <c r="C124" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B125" t="s">
+        <v>397</v>
+      </c>
+      <c r="C125" t="s">
         <v>398</v>
-      </c>
-      <c r="C125" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B126" t="s">
+        <v>399</v>
+      </c>
+      <c r="C126" t="s">
         <v>400</v>
-      </c>
-      <c r="C126" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B127" t="s">
+        <v>401</v>
+      </c>
+      <c r="C127" t="s">
         <v>402</v>
-      </c>
-      <c r="C127" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B128" t="s">
+        <v>403</v>
+      </c>
+      <c r="C128" t="s">
         <v>404</v>
-      </c>
-      <c r="C128" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B129" t="s">
+        <v>405</v>
+      </c>
+      <c r="C129" t="s">
         <v>406</v>
-      </c>
-      <c r="C129" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B130" t="s">
+        <v>407</v>
+      </c>
+      <c r="C130" t="s">
         <v>408</v>
-      </c>
-      <c r="C130" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B131" t="s">
+        <v>409</v>
+      </c>
+      <c r="C131" t="s">
         <v>410</v>
-      </c>
-      <c r="C131" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B132" t="s">
+        <v>411</v>
+      </c>
+      <c r="C132" t="s">
         <v>412</v>
-      </c>
-      <c r="C132" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B133" t="s">
+        <v>413</v>
+      </c>
+      <c r="C133" t="s">
         <v>414</v>
-      </c>
-      <c r="C133" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B134" t="s">
+        <v>415</v>
+      </c>
+      <c r="C134" t="s">
         <v>416</v>
-      </c>
-      <c r="C134" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B135" t="s">
+        <v>417</v>
+      </c>
+      <c r="C135" t="s">
         <v>418</v>
-      </c>
-      <c r="C135" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B136" t="s">
+        <v>419</v>
+      </c>
+      <c r="C136" t="s">
         <v>420</v>
-      </c>
-      <c r="C136" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B137" t="s">
+        <v>421</v>
+      </c>
+      <c r="C137" t="s">
         <v>422</v>
-      </c>
-      <c r="C137" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B138" t="s">
+        <v>423</v>
+      </c>
+      <c r="C138" t="s">
         <v>424</v>
-      </c>
-      <c r="C138" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B139" t="s">
+        <v>425</v>
+      </c>
+      <c r="C139" t="s">
         <v>426</v>
-      </c>
-      <c r="C139" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B140" t="s">
+        <v>427</v>
+      </c>
+      <c r="C140" t="s">
         <v>428</v>
-      </c>
-      <c r="C140" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B141" t="s">
+        <v>429</v>
+      </c>
+      <c r="C141" t="s">
         <v>430</v>
-      </c>
-      <c r="C141" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B142" t="s">
+        <v>431</v>
+      </c>
+      <c r="C142" t="s">
         <v>432</v>
-      </c>
-      <c r="C142" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B143" t="s">
+        <v>433</v>
+      </c>
+      <c r="C143" t="s">
         <v>434</v>
-      </c>
-      <c r="C143" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B144" t="s">
+        <v>435</v>
+      </c>
+      <c r="C144" t="s">
         <v>436</v>
-      </c>
-      <c r="C144" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B145" t="s">
+        <v>437</v>
+      </c>
+      <c r="C145" t="s">
         <v>438</v>
-      </c>
-      <c r="C145" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B146" t="s">
+        <v>439</v>
+      </c>
+      <c r="C146" t="s">
         <v>440</v>
-      </c>
-      <c r="C146" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B147" t="s">
+        <v>441</v>
+      </c>
+      <c r="C147" t="s">
         <v>442</v>
-      </c>
-      <c r="C147" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B148" t="s">
+        <v>443</v>
+      </c>
+      <c r="C148" t="s">
         <v>444</v>
-      </c>
-      <c r="C148" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B149" t="s">
+        <v>445</v>
+      </c>
+      <c r="C149" t="s">
         <v>446</v>
-      </c>
-      <c r="C149" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B150" t="s">
+        <v>447</v>
+      </c>
+      <c r="C150" t="s">
         <v>448</v>
-      </c>
-      <c r="C150" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B151" t="s">
+        <v>449</v>
+      </c>
+      <c r="C151" t="s">
         <v>450</v>
-      </c>
-      <c r="C151" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B152" t="s">
+        <v>451</v>
+      </c>
+      <c r="C152" t="s">
         <v>452</v>
-      </c>
-      <c r="C152" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B153" t="s">
+        <v>453</v>
+      </c>
+      <c r="C153" t="s">
         <v>454</v>
-      </c>
-      <c r="C153" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B154" t="s">
+        <v>455</v>
+      </c>
+      <c r="C154" t="s">
         <v>456</v>
-      </c>
-      <c r="C154" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B155" t="s">
+        <v>457</v>
+      </c>
+      <c r="C155" t="s">
         <v>458</v>
-      </c>
-      <c r="C155" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B156" t="s">
+        <v>459</v>
+      </c>
+      <c r="C156" t="s">
         <v>460</v>
-      </c>
-      <c r="C156" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B157" t="s">
+        <v>461</v>
+      </c>
+      <c r="C157" t="s">
         <v>462</v>
-      </c>
-      <c r="C157" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B158" t="s">
+        <v>463</v>
+      </c>
+      <c r="C158" t="s">
         <v>464</v>
-      </c>
-      <c r="C158" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B159" t="s">
+        <v>465</v>
+      </c>
+      <c r="C159" t="s">
         <v>466</v>
-      </c>
-      <c r="C159" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B160" t="s">
+        <v>467</v>
+      </c>
+      <c r="C160" t="s">
         <v>468</v>
-      </c>
-      <c r="C160" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B161" t="s">
+        <v>469</v>
+      </c>
+      <c r="C161" t="s">
         <v>470</v>
-      </c>
-      <c r="C161" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B162" t="s">
+        <v>471</v>
+      </c>
+      <c r="C162" t="s">
         <v>472</v>
-      </c>
-      <c r="C162" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B163" t="s">
+        <v>473</v>
+      </c>
+      <c r="C163" t="s">
         <v>474</v>
-      </c>
-      <c r="C163" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B164" t="s">
+        <v>475</v>
+      </c>
+      <c r="C164" t="s">
         <v>476</v>
-      </c>
-      <c r="C164" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B165" t="s">
+        <v>477</v>
+      </c>
+      <c r="C165" t="s">
         <v>478</v>
-      </c>
-      <c r="C165" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B166" t="s">
+        <v>479</v>
+      </c>
+      <c r="C166" t="s">
         <v>480</v>
-      </c>
-      <c r="C166" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B167" t="s">
+        <v>481</v>
+      </c>
+      <c r="C167" t="s">
         <v>482</v>
-      </c>
-      <c r="C167" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B168" t="s">
+        <v>483</v>
+      </c>
+      <c r="C168" t="s">
         <v>484</v>
-      </c>
-      <c r="C168" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B169" t="s">
+        <v>485</v>
+      </c>
+      <c r="C169" t="s">
         <v>486</v>
-      </c>
-      <c r="C169" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B170" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C170" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B171" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C171" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B172" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C172" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B173" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C173" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>